<commit_message>
Ajout section Formation, rapport stage J&A, correction CV
</commit_message>
<xml_diff>
--- a/pdf/annexe-bts.xlsx
+++ b/pdf/annexe-bts.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33658\Desktop\PortfolioAZiz\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9899D-BFDB-4477-ABF7-D82B50535297}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64FCC00-B1EA-4AB8-A746-582AAF444FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$38</definedName>
   </definedNames>
-  <calcPr calcId="101716"/>
+  <calcPr calcId="101716" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="70">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -122,9 +122,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Création infrastructure réseau</t>
-  </si>
-  <si>
     <t>Organisation à l'aide d'un diagramme de Gantt</t>
   </si>
   <si>
@@ -153,19 +150,10 @@
 (Javascript, html, css)</t>
   </si>
   <si>
-    <t>Réalisation cahier de charge (Projet jeu Devine le nombre)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Réalisation d'un cahier des charges 
 </t>
   </si>
   <si>
-    <t>Adresse URL du portfolio : https://azizbenyamina94.wordpress.com/?ref=spelling</t>
-  </si>
-  <si>
-    <t>NOM et prénom : BENYAMINA-HOUARI</t>
-  </si>
-  <si>
     <t>X SISR</t>
   </si>
   <si>
@@ -185,6 +173,87 @@
   </si>
   <si>
     <t>Déploiement de l’outil Kanboard pour la gestion des projets au sein d’une petite structure.</t>
+  </si>
+  <si>
+    <t>Durcissement et audit de sécurité d'un serveur Debian 13 avec Lynis, UFW et Fail2Ban.</t>
+  </si>
+  <si>
+    <t>Mise en place d'une infrastructure Docker sécurisée avec segmentation réseau et sauvegardes automatisées.</t>
+  </si>
+  <si>
+    <t>Déploiement d'une stack d'authentification sur Kubernetes avec Helm et résolution d'incidents Ingress.</t>
+  </si>
+  <si>
+    <t>Sécurisation d'un cluster K3s par le chiffrement au repos et la gestion des secrets via Sealed Secrets.</t>
+  </si>
+  <si>
+    <t>Installation d'un serveur GitLab CE sécurisé par un VPN WireGuard et automatisation des sauvegardes.</t>
+  </si>
+  <si>
+    <t>Création de guides de sensibilisation sur la gestion des mots de passe, le MFA et le phishing</t>
+  </si>
+  <si>
+    <t>Installation d'Auditd et AIDE pour surveiller en temps réel les modifications critiques du système de fichiers</t>
+  </si>
+  <si>
+    <t>Gestion du parc d'impression : Installation et configuration d'imprimantes HP sur serveur d'impression avec gestion des pilotes et des ports TCP/IP.</t>
+  </si>
+  <si>
+    <t>Maintenance de la téléphonie IP : Support et mise en service de terminaux IP Avaya et Ascom au sein d'une infrastructure IPABX hospitalière.</t>
+  </si>
+  <si>
+    <t>Segmentation réseau (Switch) : Configuration d'un commutateur Enterasys incluant la création de VLAN (Backup), l'activation du SSH et la sécurisation des accès.</t>
+  </si>
+  <si>
+    <t>Déploiement système (WDS) : Préparation et capture d'une image de référence Windows 11 pour automatiser le déploiement des postes via le réseau (PXE).</t>
+  </si>
+  <si>
+    <t>Inventaire automatisé (GLPI) : Déploiement de l'agent GLPI sur les postes clients pour assurer la remontée automatique de l'inventaire matériel et logiciel.</t>
+  </si>
+  <si>
+    <t>Optimisation du stockage LVM et migration de VM critique (Cluster Proxmox</t>
+  </si>
+  <si>
+    <t>Configuration des routeurs et switches avec segmentation par VLAN pour isoler les flux.</t>
+  </si>
+  <si>
+    <t>Projet Mairie : Segmentation réseau et sécurisation des accès Wi-Fi/Filaires par VLAN pour isoler les services administratifs et publics.</t>
+  </si>
+  <si>
+    <t>Activation et configuration des journaux d'audit (audit logs) pour tracer chaque action effectuée sur le cluster K3s.</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://itzazizo.github.io/PortfolioAziz/</t>
+  </si>
+  <si>
+    <t>NOM et prénom : BENYAMINA-HOUARI Aziz</t>
+  </si>
+  <si>
+    <t>10/09/2024 au 11/09/2024</t>
+  </si>
+  <si>
+    <t>06/09/2024 au 06/12/2024</t>
+  </si>
+  <si>
+    <t>Création infrastructure réseau ( Packet tracer)</t>
+  </si>
+  <si>
+    <t>10/2025-11/2025</t>
+  </si>
+  <si>
+    <t>Installation et configuration d'un système IDS/IPS pour la détection et le blocage proactif d'intrusions sur le réseau.</t>
+  </si>
+  <si>
+    <t>Planification des activités et suivi des ressources à l'aide d'un diagramme de Gantt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Installation d'un pare-feu pfSense, configuration du NAT sortant et mise en place de règles de filtrage LAN/WAN.</t>
+  </si>
+  <si>
+    <t>02/12/2024 au 24/01/2025</t>
+  </si>
+  <si>
+    <t>Mise en place de l'inventaire automatisé via le déploiement d'agents GLPI par GPO  sur un Active Directory.</t>
   </si>
 </sst>
 </file>
@@ -194,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -257,21 +326,61 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial1"/>
+    </font>
+    <font>
       <b/>
-      <sz val="28"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -391,36 +500,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
     <border diagonalDown="1">
       <left style="medium">
         <color theme="2" tint="-0.749992370372631"/>
@@ -657,12 +736,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF4A452A"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF4A452A"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -670,13 +820,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -685,23 +829,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -709,113 +841,139 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Default" xfId="2" xr:uid="{5BCF07CE-08FA-457D-A2BD-ACC8AC01EAD6}"/>
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -833,9 +991,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -873,9 +1031,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -908,26 +1066,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -960,26 +1101,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1156,139 +1280,139 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ85"/>
+  <dimension ref="A1:AQ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="1" customWidth="1"/>
-    <col min="3" max="8" width="18.7109375" style="1" customWidth="1"/>
-    <col min="9" max="43" width="11.42578125" customWidth="1"/>
-    <col min="44" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="1" customWidth="1"/>
+    <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
+    <col min="9" max="43" width="11.44140625" customWidth="1"/>
+    <col min="44" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:43" ht="39.9" customHeight="1">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="34"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1">
+      <c r="A2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-    </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="49" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:43" ht="39.9" customHeight="1">
+      <c r="A3" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="50"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="37"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:43" ht="39.9" customHeight="1">
+      <c r="A4" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="14" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="22" t="s">
+      <c r="G4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A5" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1">
+      <c r="A6" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="23" t="s">
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1">
+      <c r="A7" s="45"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="12" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
@@ -1327,17 +1451,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="72" customHeight="1" thickBot="1">
+      <c r="A8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1374,23 +1498,21 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="29"/>
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1427,27 +1549,25 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="29"/>
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="18"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1484,21 +1604,21 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="29" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18" t="s">
         <v>25</v>
       </c>
       <c r="I11"/>
@@ -1537,23 +1657,23 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="29"/>
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1590,23 +1710,25 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="8" t="s">
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="29"/>
+      <c r="B13" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="18"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1643,23 +1765,23 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="29"/>
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1696,23 +1818,23 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="29"/>
+      <c r="C15" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="18"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1749,23 +1871,23 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="21.6" thickBot="1">
+      <c r="A16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="29"/>
+      <c r="D16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1802,23 +1924,29 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="29"/>
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1855,27 +1983,25 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="31" t="s">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="18" t="s">
         <v>25</v>
       </c>
       <c r="I18"/>
@@ -1914,29 +2040,23 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>25</v>
-      </c>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="18"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1973,25 +2093,27 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="29"/>
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -2028,27 +2150,25 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="29" t="s">
-        <v>25</v>
-      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="18"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -2085,26 +2205,28 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="29" t="s">
-        <v>25</v>
+      <c r="D22" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
@@ -2142,17 +2264,23 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="29"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="24">
+        <v>45901</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="18"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2189,15 +2317,21 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="29"/>
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="25">
+        <v>46327</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="18"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2234,15 +2368,25 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="17"/>
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="24">
+        <v>46054</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="18"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2279,15 +2423,19 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="28"/>
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="24">
+        <v>45901</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2324,15 +2472,25 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="17"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A27" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="24">
+        <v>46054</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="18"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2369,15 +2527,25 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="17"/>
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A28" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="24">
+        <v>46054</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="18"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2414,15 +2582,23 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="17"/>
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="39" customHeight="1" thickBot="1">
+      <c r="A29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="18"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2459,15 +2635,17 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="17"/>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A30" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2504,17 +2682,23 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="17"/>
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A31" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="15"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2551,15 +2735,21 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="19"/>
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="42" thickBot="1">
+      <c r="A32" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="15"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2596,15 +2786,21 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="21"/>
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="15"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2641,103 +2837,403 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="10"/>
-    </row>
-    <row r="36" spans="1:43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
-    </row>
-    <row r="37" spans="1:43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
-    </row>
-    <row r="38" spans="1:43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-    </row>
-    <row r="39" spans="1:43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-    </row>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80"/>
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="D80"/>
-      <c r="E80"/>
-      <c r="F80"/>
-      <c r="G80"/>
-      <c r="H80"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A34" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="15"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+      <c r="Z34"/>
+      <c r="AA34"/>
+      <c r="AB34"/>
+      <c r="AC34"/>
+      <c r="AD34"/>
+      <c r="AE34"/>
+      <c r="AF34"/>
+      <c r="AG34"/>
+      <c r="AH34"/>
+      <c r="AI34"/>
+      <c r="AJ34"/>
+      <c r="AK34"/>
+      <c r="AL34"/>
+      <c r="AM34"/>
+      <c r="AN34"/>
+      <c r="AO34"/>
+      <c r="AP34"/>
+      <c r="AQ34"/>
+    </row>
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A35" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="15"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+      <c r="AB35"/>
+      <c r="AC35"/>
+      <c r="AD35"/>
+      <c r="AE35"/>
+      <c r="AF35"/>
+      <c r="AG35"/>
+      <c r="AH35"/>
+      <c r="AI35"/>
+      <c r="AJ35"/>
+      <c r="AK35"/>
+      <c r="AL35"/>
+      <c r="AM35"/>
+      <c r="AN35"/>
+      <c r="AO35"/>
+      <c r="AP35"/>
+      <c r="AQ35"/>
+    </row>
+    <row r="36" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1">
+      <c r="A36" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="43"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AJ36"/>
+      <c r="AK36"/>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+    </row>
+    <row r="37" spans="1:43" s="2" customFormat="1" ht="28.2" customHeight="1" thickBot="1">
+      <c r="A37" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37"/>
+      <c r="AC37"/>
+      <c r="AD37"/>
+      <c r="AE37"/>
+      <c r="AF37"/>
+      <c r="AG37"/>
+      <c r="AH37"/>
+      <c r="AI37"/>
+      <c r="AJ37"/>
+      <c r="AK37"/>
+      <c r="AL37"/>
+      <c r="AM37"/>
+      <c r="AN37"/>
+      <c r="AO37"/>
+      <c r="AP37"/>
+      <c r="AQ37"/>
+    </row>
+    <row r="38" spans="1:43" customFormat="1" ht="41.4" customHeight="1" thickBot="1">
+      <c r="A38" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="16"/>
+    </row>
+    <row r="39" spans="1:43" customFormat="1" ht="36.6" customHeight="1" thickBot="1">
+      <c r="A39" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:43" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1">
+      <c r="A40" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:43" customFormat="1" ht="43.8" customHeight="1" thickBot="1">
+      <c r="A41" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="1:43" customFormat="1" ht="52.2" customHeight="1" thickBot="1">
+      <c r="A42" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="27"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:43" customFormat="1" ht="33" customHeight="1">
+      <c r="A43" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="27"/>
+      <c r="C43" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:43" customFormat="1" ht="36" customHeight="1" thickBot="1">
+      <c r="A44" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="28"/>
+      <c r="C44" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" s="23"/>
+    </row>
+    <row r="45" spans="1:43" customFormat="1" ht="16.2" thickBot="1">
+      <c r="B45" s="20"/>
+    </row>
+    <row r="46" spans="1:43" customFormat="1"/>
+    <row r="47" spans="1:43" customFormat="1"/>
+    <row r="48" spans="1:43" customFormat="1"/>
+    <row r="49" customFormat="1"/>
+    <row r="50" customFormat="1"/>
+    <row r="51" customFormat="1"/>
+    <row r="52" customFormat="1"/>
+    <row r="53" customFormat="1"/>
+    <row r="54" customFormat="1"/>
+    <row r="55" customFormat="1"/>
+    <row r="56" customFormat="1"/>
+    <row r="57" customFormat="1"/>
+    <row r="58" customFormat="1"/>
+    <row r="59" customFormat="1"/>
+    <row r="60" customFormat="1"/>
+    <row r="61" customFormat="1"/>
+    <row r="62" customFormat="1"/>
+    <row r="63" customFormat="1"/>
+    <row r="64" customFormat="1"/>
+    <row r="65" customFormat="1"/>
+    <row r="66" customFormat="1"/>
+    <row r="67" customFormat="1"/>
+    <row r="68" customFormat="1"/>
+    <row r="69" customFormat="1"/>
+    <row r="70" customFormat="1"/>
+    <row r="71" customFormat="1"/>
+    <row r="72" customFormat="1"/>
+    <row r="73" customFormat="1"/>
+    <row r="74" customFormat="1"/>
+    <row r="75" customFormat="1"/>
+    <row r="76" customFormat="1"/>
+    <row r="77" customFormat="1"/>
+    <row r="78" customFormat="1"/>
+    <row r="79" customFormat="1"/>
+    <row r="80" customFormat="1"/>
+    <row r="81" spans="1:8" customFormat="1"/>
+    <row r="82" spans="1:8" customFormat="1"/>
+    <row r="83" spans="1:8" customFormat="1"/>
+    <row r="84" spans="1:8">
       <c r="A84"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B84"/>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84"/>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85"/>
     </row>
+    <row r="86" spans="1:8">
+      <c r="A86"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87"/>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="B37:B44"/>
+    <mergeCell ref="B31:B35"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A36:H36"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2747,7 +3243,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="46" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout section Technologies avec slider anime et filtres interactifs
</commit_message>
<xml_diff>
--- a/pdf/annexe-bts.xlsx
+++ b/pdf/annexe-bts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33658\Desktop\PortfolioAZiz\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64FCC00-B1EA-4AB8-A746-582AAF444FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535BE265-AB54-43FE-8533-220E40E8C966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$38</definedName>
+    <definedName name="BTS_SERVICES_INFORMATIQUES_AUX_ORGANISATIONS">'Tableau de synthèse Épreuve E4'!$A$1:$H$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$45</definedName>
   </definedNames>
   <calcPr calcId="101716" iterateDelta="1E-4"/>
 </workbook>
@@ -1282,8 +1283,8 @@
   </sheetPr>
   <dimension ref="A1:AQ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2"/>
@@ -3243,7 +3244,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="46" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>